<commit_message>
update literaturverzeichnis + gedanken
</commit_message>
<xml_diff>
--- a/03_thesis/Literaturverzeichnis.xlsx
+++ b/03_thesis/Literaturverzeichnis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Desktop/FoodAnalyser/03_thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9555D7E2-7C81-CA4F-B08D-7B7A0D87DF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F677721-11D5-0043-B162-59F7D099FE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="500" windowWidth="67500" windowHeight="10940" xr2:uid="{3701A8F3-D4B0-D940-B81D-3D1CB3DADD6F}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="67420" windowHeight="10940" xr2:uid="{3701A8F3-D4B0-D940-B81D-3D1CB3DADD6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Literatur" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1851" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="636">
   <si>
     <t>Nr</t>
   </si>
@@ -1518,9 +1518,6 @@
     <t>Umkreis</t>
   </si>
   <si>
-    <t>4, 6</t>
-  </si>
-  <si>
     <t>Umkugel</t>
   </si>
   <si>
@@ -1549,6 +1546,408 @@
   </si>
   <si>
     <t>194</t>
+  </si>
+  <si>
+    <t>162-163</t>
+  </si>
+  <si>
+    <t>Dreidimensionales Mesh mit Tetraeder und Umkugel</t>
+  </si>
+  <si>
+    <t>mesh_tetraeder_umkugel.svg</t>
+  </si>
+  <si>
+    <t>https://www.google.de/books/edition/Computational_Engineering_Introduction_t/bEw5EAAAQBAJ?hl=de&amp;gbpv=1</t>
+  </si>
+  <si>
+    <t>Schematischer Ablauf des Bowyer-Watson Algorithmus</t>
+  </si>
+  <si>
+    <t>delaunay_triangulation_1.svg; delaunay_triangulation_2.svg</t>
+  </si>
+  <si>
+    <t>Schäfer, M.</t>
+  </si>
+  <si>
+    <t>Schäfer, Michael</t>
+  </si>
+  <si>
+    <t>77-79</t>
+  </si>
+  <si>
+    <t>Computational Engineering - Introduction to Numerical Methods</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>9783030760274</t>
+  </si>
+  <si>
+    <t>4, 6-7</t>
+  </si>
+  <si>
+    <t>Gesamtvolumen eines 3D Meshs</t>
+  </si>
+  <si>
+    <t>Berechnung des Gesamtvolumens eines 3D Meshs</t>
+  </si>
+  <si>
+    <t>Berechnung des Volumens eines Tetraeders</t>
+  </si>
+  <si>
+    <t>Weisstein, Eric W.</t>
+  </si>
+  <si>
+    <t>Weisstein, E.</t>
+  </si>
+  <si>
+    <t>MathWorld--A Wolfram Web Resource.</t>
+  </si>
+  <si>
+    <t>o. S.</t>
+  </si>
+  <si>
+    <t>Tetrahedron</t>
+  </si>
+  <si>
+    <t>https://mathworld.wolfram.com/Tetrahedron.html</t>
+  </si>
+  <si>
+    <t>793-796</t>
+  </si>
+  <si>
+    <t>2018_Differenzmethode_Volume_estimation_of_strawberries_mushrooms_and_to.pdf</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/327132182_Volume_estimation_of_strawberries_mushrooms_and_tomatoes_with_a_machine_vision_system</t>
+  </si>
+  <si>
+    <t>Differenzmethode</t>
+  </si>
+  <si>
+    <t>Volume estimation of strawberries, mushrooms, and tomatoes with a machine vision system</t>
+  </si>
+  <si>
+    <t>Concha-Meyer, Aníbal; Eifert, Joseph; Wang, Hengjian; Sanglay, Gabriel</t>
+  </si>
+  <si>
+    <t>Concha-Meyer, A. et al.</t>
+  </si>
+  <si>
+    <t>10.1080/10942912.2018.1508156</t>
+  </si>
+  <si>
+    <t>International Journal of Food Properties, vol. 21, no. 1</t>
+  </si>
+  <si>
+    <t>1868-1869</t>
+  </si>
+  <si>
+    <t>2017_ManualforBuildingTreeVolumeandBiomassAllometricEquationforBangladesh.pdf</t>
+  </si>
+  <si>
+    <t>Hossain, Mahmood; Siddique, Mohammad Raqibul Hasan; Abdullah, S.M.R.; Akhter, Mariam; SMZ, Islam</t>
+  </si>
+  <si>
+    <t>Bangladesh Forest Department</t>
+  </si>
+  <si>
+    <t>differenzmethode.svg</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/322593979_MANUAL_FOR_BUILDING_TREE_VOLUME_AND_BIOMASS_ALLOMETRIC_EQUATION_FOR_BANGLADESH</t>
+  </si>
+  <si>
+    <t>Hossain, M. et al.</t>
+  </si>
+  <si>
+    <t>978-984-34-2711-3</t>
+  </si>
+  <si>
+    <t>Manual for building tree volume and biomass allometric equation for bangladesh</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>Photogrammetry-Based Volume Measurement Framework for the Particle Density Estimation of LECA</t>
+  </si>
+  <si>
+    <t>2022_Differenzmethode_Archimedes.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/1996-1944/15/15/5388</t>
+  </si>
+  <si>
+    <t>10.3390/ma15155388</t>
+  </si>
+  <si>
+    <t>Brzeziński, Karol; Duda, Adam; Styk, Adam; Kowaluk, Tomasz</t>
+  </si>
+  <si>
+    <t>Brzeziński, K. et al.</t>
+  </si>
+  <si>
+    <t>MDPI, Materials, vol. 15, no. 15</t>
+  </si>
+  <si>
+    <t>Bundle Adjustment - A Modern Synthesis</t>
+  </si>
+  <si>
+    <t>10.1007/3-540-44480-7_21</t>
+  </si>
+  <si>
+    <t>Triggs, Bill; McLauchlan, Philip F.; Hartley, Richard; Fitzgibbon, Andrew William</t>
+  </si>
+  <si>
+    <t>Triggs, B. et al.</t>
+  </si>
+  <si>
+    <t>Triggs, B., Zisserman, A., Szeliski, R. (eds) Vision Algorithms: Theory and Practice. IWVA 1999. Lecture Notes in Computer Science, vol 1883. Springer, Berlin, Heidelberg</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/3-540-44480-7_21#citeas</t>
+  </si>
+  <si>
+    <t>2000_Triggs.pdf</t>
+  </si>
+  <si>
+    <t>298-300</t>
+  </si>
+  <si>
+    <t>bundle adjustment</t>
+  </si>
+  <si>
+    <t>299, 304-305</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/11744023_32</t>
+  </si>
+  <si>
+    <t>Primärquelle_SURF.pdf</t>
+  </si>
+  <si>
+    <t>SURF: Speeded Up Robust Features</t>
+  </si>
+  <si>
+    <t>SURF</t>
+  </si>
+  <si>
+    <t>10.1007/11744023_32</t>
+  </si>
+  <si>
+    <t>Bay, Herbert; Tuytelaars, Tinne; Van Gool, Luc</t>
+  </si>
+  <si>
+    <t>Bay, H. et al.</t>
+  </si>
+  <si>
+    <t>Leonardis, A., Bischof, H., Pinz, A. (eds) Computer Vision – ECCV 2006. ECCV 2006. Lecture Notes in Computer Science, vol 3951. Springer, Berlin, Heidelberg</t>
+  </si>
+  <si>
+    <t>978-3-540-33832-1</t>
+  </si>
+  <si>
+    <t>404-417</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>2D object recognition: a comparative analysis of SIFT, SURF and ORB feature descriptors</t>
+  </si>
+  <si>
+    <t>SIFT_vs_SURF_vs_ORB.pdf</t>
+  </si>
+  <si>
+    <t>Bansal, Monika; Kumar, Munish; Kumar, Manish</t>
+  </si>
+  <si>
+    <t>Bansal, M. et al.</t>
+  </si>
+  <si>
+    <t>10.1007/s11042-021-10646-0</t>
+  </si>
+  <si>
+    <t>SIFT vs. SURF</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11042-021-10646-0</t>
+  </si>
+  <si>
+    <t>Multimedia Tools and Applications, vol. 80</t>
+  </si>
+  <si>
+    <t>18843-18844</t>
+  </si>
+  <si>
+    <t>Accurate, Dense, and Robust Multiview Stereopsis</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/44683582_Accurate_Dense_and_Robust_Multiview_Stereopsis</t>
+  </si>
+  <si>
+    <t>PMVS</t>
+  </si>
+  <si>
+    <t>2010_PMVS.pdf</t>
+  </si>
+  <si>
+    <t>10.1109/TPAMI.2009.161</t>
+  </si>
+  <si>
+    <t>Furukawa, Yasutaka; Ponce, Jean</t>
+  </si>
+  <si>
+    <t>Furukawa, Y.; Ponce, J.</t>
+  </si>
+  <si>
+    <t>IEEE transactions on pattern analysis and machine intelligence, vol. 32, no. 8</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>1, 3-4</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2076-3417/12/9/4581</t>
+  </si>
+  <si>
+    <t>applsci-12-04581-v3.pdf</t>
+  </si>
+  <si>
+    <t>Multi-Scale Upsampling GAN Based Hole-Filling Framework for High-Quality 3D Cultural Heritage Artifacts</t>
+  </si>
+  <si>
+    <t>hole filling methods</t>
+  </si>
+  <si>
+    <t>10.3390/app12094581</t>
+  </si>
+  <si>
+    <t>MDPI, Applied Sciences, vol. 12, no. 9</t>
+  </si>
+  <si>
+    <t>Ren, Yong; Chu, Tong; Jiao, Yifei; Zhou, Mingquan; Geng, Guohua; Li, Kang; Cao, Xin</t>
+  </si>
+  <si>
+    <t>Ren, Y. et al.</t>
+  </si>
+  <si>
+    <t>Wang, Xinying; Xu, Dikai; Gu, Fangming</t>
+  </si>
+  <si>
+    <t>Wang, X. et al.</t>
+  </si>
+  <si>
+    <t>10.1109/ACCESS.2020.3024288</t>
+  </si>
+  <si>
+    <t>3D-DCGAN</t>
+  </si>
+  <si>
+    <t>3D Model Inpainting Based on 3D Deep Convolutional Generative Adversarial Network</t>
+  </si>
+  <si>
+    <t>3D_Model_Inpainting_Based_on_3D_Deep_Convolutional_Generative_Adversarial_Network.pdf</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9197608</t>
+  </si>
+  <si>
+    <t>IEEE Access, vol. 8</t>
+  </si>
+  <si>
+    <t>170355-170363</t>
+  </si>
+  <si>
+    <t>1-14</t>
+  </si>
+  <si>
+    <t>MU-GAN</t>
+  </si>
+  <si>
+    <t>170355-170356</t>
+  </si>
+  <si>
+    <t>https://developer.apple.com/videos/wwdc2021/?q=object%20capture</t>
+  </si>
+  <si>
+    <t>WWDC21</t>
+  </si>
+  <si>
+    <t>2023-04-10</t>
+  </si>
+  <si>
+    <t>https://developer.apple.com/documentation/RealityKit/capturing-photographs-for-realitykit-object-capture</t>
+  </si>
+  <si>
+    <t>RealityKit Object Capture</t>
+  </si>
+  <si>
+    <t>https://developer.apple.com/augmented-reality/</t>
+  </si>
+  <si>
+    <t>Dive into the world of augmented reality.</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>A Head-Mounted Three Dimensional Display</t>
+  </si>
+  <si>
+    <t>Sutherland, Ivan E.</t>
+  </si>
+  <si>
+    <t>Sutherland, I.</t>
+  </si>
+  <si>
+    <t>10.1145/1476589.1476686</t>
+  </si>
+  <si>
+    <t>Primärquelle_1968_Ivan.pdf</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/1476589.1476686</t>
+  </si>
+  <si>
+    <t>Association for Computing Machinery, USA, New York</t>
+  </si>
+  <si>
+    <t>9781450378994</t>
+  </si>
+  <si>
+    <t>757-764</t>
+  </si>
+  <si>
+    <t>2022_AR.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2073-431X/11/2/28</t>
+  </si>
+  <si>
+    <t>An Overview of Augmented Reality</t>
+  </si>
+  <si>
+    <t>10.3390/computers11020028</t>
+  </si>
+  <si>
+    <t>Arena, Fabio; Collotta, Mario; Pau, Giovanni; Termine, Francesco</t>
+  </si>
+  <si>
+    <t>Arena, F. et al.</t>
+  </si>
+  <si>
+    <t>MDPI, Computers, vol. 11, no. 2</t>
+  </si>
+  <si>
+    <t>https://developer.apple.com/augmented-reality/object-capture/</t>
+  </si>
+  <si>
+    <t>Introducing Object Capture</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +2039,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1698,12 +2097,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1839,6 +2249,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2156,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DB0257-C51B-E14C-83D3-EA7E67364B51}">
   <dimension ref="A1:Q208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="145" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="145" workbookViewId="0">
+      <selection activeCell="B193" sqref="B193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8734,11 +9155,11 @@
         <v>2021</v>
       </c>
       <c r="M145" s="23" t="s">
-        <v>492</v>
+        <v>514</v>
       </c>
       <c r="N145" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. Liu, Y.; Zheng, Y., Umkreis, 2021, S. 4, 6.</v>
+        <v>Vgl. Liu, Y.; Zheng, Y., Umkreis, 2021, S. 4, 6-7.</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
@@ -8758,7 +9179,7 @@
         <v>447</v>
       </c>
       <c r="F146" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G146" s="24" t="s">
         <v>15</v>
@@ -8839,37 +9260,37 @@
         <v>51</v>
       </c>
       <c r="C148" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D148" s="24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E148" s="24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F148" s="24" t="s">
         <v>468</v>
       </c>
       <c r="G148" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="H148" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="I148" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="J148" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K148" s="24" t="s">
         <v>494</v>
-      </c>
-      <c r="H148" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I148" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="J148" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K148" s="24" t="s">
-        <v>495</v>
       </c>
       <c r="L148" s="21">
         <v>1984</v>
       </c>
       <c r="M148" s="23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N148" s="17" t="str">
         <f t="shared" si="5"/>
@@ -8884,37 +9305,37 @@
         <v>51</v>
       </c>
       <c r="C149" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D149" s="24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E149" s="24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F149" s="24" t="s">
         <v>468</v>
       </c>
       <c r="G149" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="H149" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="I149" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="J149" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K149" s="24" t="s">
         <v>494</v>
-      </c>
-      <c r="H149" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I149" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="J149" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K149" s="24" t="s">
-        <v>495</v>
       </c>
       <c r="L149" s="21">
         <v>1984</v>
       </c>
       <c r="M149" s="23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="N149" s="17" t="str">
         <f t="shared" si="5"/>
@@ -9019,37 +9440,37 @@
         <v>51</v>
       </c>
       <c r="C152" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D152" s="24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E152" s="24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F152" s="24" t="s">
         <v>468</v>
       </c>
       <c r="G152" s="24" t="s">
+        <v>493</v>
+      </c>
+      <c r="H152" s="24" t="s">
+        <v>497</v>
+      </c>
+      <c r="I152" s="24" t="s">
+        <v>496</v>
+      </c>
+      <c r="J152" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K152" s="24" t="s">
         <v>494</v>
-      </c>
-      <c r="H152" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="I152" s="24" t="s">
-        <v>497</v>
-      </c>
-      <c r="J152" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="K152" s="24" t="s">
-        <v>495</v>
       </c>
       <c r="L152" s="21">
         <v>1984</v>
       </c>
       <c r="M152" s="23" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="N152" s="17" t="str">
         <f t="shared" si="5"/>
@@ -9060,840 +9481,1806 @@
       <c r="A153" s="14">
         <v>152</v>
       </c>
-      <c r="B153" s="21"/>
-      <c r="C153" s="24"/>
-      <c r="D153" s="24"/>
-      <c r="E153" s="24"/>
-      <c r="F153" s="21"/>
-      <c r="G153" s="21"/>
-      <c r="H153" s="24"/>
-      <c r="I153" s="24"/>
-      <c r="J153" s="25"/>
-      <c r="K153" s="24"/>
-      <c r="L153" s="21"/>
-      <c r="M153" s="23"/>
+      <c r="B153" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C153" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="D153" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="E153" s="24" t="s">
+        <v>477</v>
+      </c>
+      <c r="F153" s="24" t="s">
+        <v>468</v>
+      </c>
+      <c r="G153" s="24" t="s">
+        <v>474</v>
+      </c>
+      <c r="H153" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="I153" s="24" t="s">
+        <v>473</v>
+      </c>
+      <c r="J153" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K153" s="24" t="s">
+        <v>479</v>
+      </c>
+      <c r="L153" s="21">
+        <v>1981</v>
+      </c>
+      <c r="M153" s="23" t="s">
+        <v>502</v>
+      </c>
       <c r="N153" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Bowyer, A., Bowyer-Watson Algorithmus, 1981, S. 162-163.</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="21">
         <v>153</v>
       </c>
-      <c r="B154" s="21"/>
-      <c r="C154" s="24"/>
-      <c r="D154" s="24"/>
-      <c r="E154" s="24"/>
-      <c r="F154" s="21"/>
-      <c r="G154" s="21"/>
-      <c r="H154" s="24"/>
-      <c r="I154" s="24"/>
-      <c r="J154" s="25"/>
-      <c r="K154" s="24"/>
-      <c r="L154" s="21"/>
-      <c r="M154" s="23"/>
+      <c r="B154" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C154" s="37" t="s">
+        <v>452</v>
+      </c>
+      <c r="D154" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="E154" s="24" t="s">
+        <v>451</v>
+      </c>
+      <c r="F154" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="G154" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H154" s="24" t="s">
+        <v>450</v>
+      </c>
+      <c r="I154" s="24" t="s">
+        <v>450</v>
+      </c>
+      <c r="J154" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K154" s="24" t="s">
+        <v>454</v>
+      </c>
+      <c r="L154" s="21">
+        <v>1934</v>
+      </c>
+      <c r="M154" s="23" t="s">
+        <v>524</v>
+      </c>
       <c r="N154" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Delaunay, B., Delaunay-Triangulation, 1934, S. 793-796.</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="21">
         <v>154</v>
       </c>
-      <c r="B155" s="21"/>
-      <c r="C155" s="24"/>
-      <c r="D155" s="24"/>
-      <c r="E155" s="24"/>
-      <c r="F155" s="21"/>
-      <c r="G155" s="21"/>
-      <c r="H155" s="24"/>
-      <c r="I155" s="24"/>
-      <c r="J155" s="25"/>
-      <c r="K155" s="24"/>
-      <c r="L155" s="21"/>
-      <c r="M155" s="23"/>
+      <c r="B155" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C155" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="D155" s="24" t="s">
+        <v>470</v>
+      </c>
+      <c r="E155" s="24" t="s">
+        <v>469</v>
+      </c>
+      <c r="F155" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="G155" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="H155" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="I155" s="24" t="s">
+        <v>463</v>
+      </c>
+      <c r="J155" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K155" s="24" t="s">
+        <v>466</v>
+      </c>
+      <c r="L155" s="21">
+        <v>2021</v>
+      </c>
+      <c r="M155" s="23" t="s">
+        <v>268</v>
+      </c>
       <c r="N155" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Liu, Y.; Zheng, Y., Gesamtvolumen eines 3D Meshs, 2021, S. 3.</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="14">
         <v>155</v>
       </c>
-      <c r="B156" s="21"/>
-      <c r="C156" s="24"/>
-      <c r="D156" s="24"/>
-      <c r="E156" s="24"/>
-      <c r="F156" s="21"/>
-      <c r="G156" s="21"/>
-      <c r="H156" s="24"/>
-      <c r="I156" s="24"/>
-      <c r="J156" s="25"/>
-      <c r="K156" s="24"/>
-      <c r="L156" s="21"/>
-      <c r="M156" s="23"/>
+      <c r="B156" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C156" s="37" t="s">
+        <v>471</v>
+      </c>
+      <c r="D156" s="24" t="s">
+        <v>470</v>
+      </c>
+      <c r="E156" s="24" t="s">
+        <v>469</v>
+      </c>
+      <c r="F156" s="24" t="s">
+        <v>515</v>
+      </c>
+      <c r="G156" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="H156" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="I156" s="24" t="s">
+        <v>463</v>
+      </c>
+      <c r="J156" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K156" s="24" t="s">
+        <v>466</v>
+      </c>
+      <c r="L156" s="21">
+        <v>2021</v>
+      </c>
+      <c r="M156" s="23" t="s">
+        <v>268</v>
+      </c>
       <c r="N156" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Liu, Y.; Zheng, Y., Gesamtvolumen eines 3D Meshs, 2021, S. 3.</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="21">
         <v>156</v>
       </c>
-      <c r="B157" s="21"/>
-      <c r="C157" s="24"/>
-      <c r="D157" s="24"/>
-      <c r="E157" s="24"/>
-      <c r="F157" s="21"/>
-      <c r="G157" s="21"/>
-      <c r="H157" s="24"/>
-      <c r="I157" s="24"/>
-      <c r="J157" s="25"/>
-      <c r="K157" s="24"/>
-      <c r="L157" s="21"/>
-      <c r="M157" s="23"/>
+      <c r="B157" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C157" s="37" t="s">
+        <v>526</v>
+      </c>
+      <c r="D157" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="E157" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F157" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G157" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="H157" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="I157" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="J157" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K157" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="L157" s="21">
+        <v>2018</v>
+      </c>
+      <c r="M157" s="23" t="s">
+        <v>533</v>
+      </c>
       <c r="N157" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Concha-Meyer, A. et al., Differenzmethode, 2018, S. 1868-1869.</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="21">
         <v>157</v>
       </c>
-      <c r="B158" s="21"/>
-      <c r="C158" s="24"/>
-      <c r="D158" s="24"/>
-      <c r="E158" s="24"/>
-      <c r="F158" s="21"/>
-      <c r="G158" s="21"/>
-      <c r="H158" s="24"/>
-      <c r="I158" s="24"/>
-      <c r="J158" s="25"/>
-      <c r="K158" s="24"/>
-      <c r="L158" s="21"/>
-      <c r="M158" s="23"/>
+      <c r="B158" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C158" s="37" t="s">
+        <v>526</v>
+      </c>
+      <c r="D158" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="E158" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F158" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G158" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="H158" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="I158" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="J158" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K158" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="L158" s="21">
+        <v>2018</v>
+      </c>
+      <c r="M158" s="23" t="s">
+        <v>533</v>
+      </c>
       <c r="N158" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Concha-Meyer, A. et al., Differenzmethode, 2018, S. 1868-1869.</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="14">
         <v>158</v>
       </c>
-      <c r="B159" s="21"/>
-      <c r="C159" s="24"/>
-      <c r="D159" s="24"/>
-      <c r="E159" s="24"/>
-      <c r="F159" s="21"/>
-      <c r="G159" s="21"/>
-      <c r="H159" s="24"/>
-      <c r="I159" s="24"/>
-      <c r="J159" s="25"/>
-      <c r="K159" s="24"/>
-      <c r="L159" s="21"/>
-      <c r="M159" s="23"/>
+      <c r="B159" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C159" s="37" t="s">
+        <v>526</v>
+      </c>
+      <c r="D159" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="E159" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F159" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G159" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="H159" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="I159" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="J159" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K159" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="L159" s="21">
+        <v>2018</v>
+      </c>
+      <c r="M159" s="23" t="s">
+        <v>533</v>
+      </c>
       <c r="N159" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Concha-Meyer, A. et al., Differenzmethode, 2018, S. 1868-1869.</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" s="21">
         <v>159</v>
       </c>
-      <c r="B160" s="21"/>
-      <c r="C160" s="24"/>
-      <c r="D160" s="24"/>
-      <c r="E160" s="24"/>
-      <c r="F160" s="21"/>
-      <c r="G160" s="21"/>
-      <c r="H160" s="24"/>
-      <c r="I160" s="24"/>
-      <c r="J160" s="25"/>
-      <c r="K160" s="24"/>
-      <c r="L160" s="21"/>
-      <c r="M160" s="23"/>
+      <c r="B160" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C160" s="37" t="s">
+        <v>526</v>
+      </c>
+      <c r="D160" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="E160" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F160" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G160" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="H160" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="I160" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="J160" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K160" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="L160" s="21">
+        <v>2018</v>
+      </c>
+      <c r="M160" s="23" t="s">
+        <v>533</v>
+      </c>
       <c r="N160" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Concha-Meyer, A. et al., Differenzmethode, 2018, S. 1868-1869.</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" s="21">
         <v>160</v>
       </c>
-      <c r="B161" s="21"/>
-      <c r="C161" s="24"/>
-      <c r="D161" s="24"/>
-      <c r="E161" s="24"/>
-      <c r="F161" s="21"/>
-      <c r="G161" s="21"/>
-      <c r="H161" s="24"/>
-      <c r="I161" s="24"/>
-      <c r="J161" s="25"/>
-      <c r="K161" s="24"/>
-      <c r="L161" s="21"/>
-      <c r="M161" s="23"/>
+      <c r="B161" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C161" s="37" t="s">
+        <v>545</v>
+      </c>
+      <c r="D161" s="24" t="s">
+        <v>544</v>
+      </c>
+      <c r="E161" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="F161" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G161" s="24" t="s">
+        <v>546</v>
+      </c>
+      <c r="H161" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="I161" s="24" t="s">
+        <v>547</v>
+      </c>
+      <c r="J161" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K161" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="L161" s="21">
+        <v>2022</v>
+      </c>
+      <c r="M161" s="23" t="s">
+        <v>542</v>
+      </c>
       <c r="N161" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Brzeziński, K. et al., Differenzmethode, 2022, S. 7-8.</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" s="14">
         <v>161</v>
       </c>
-      <c r="B162" s="21"/>
-      <c r="C162" s="24"/>
-      <c r="D162" s="24"/>
-      <c r="E162" s="24"/>
-      <c r="F162" s="21"/>
-      <c r="G162" s="21"/>
-      <c r="H162" s="24"/>
-      <c r="I162" s="24"/>
-      <c r="J162" s="25"/>
-      <c r="K162" s="24"/>
-      <c r="L162" s="21"/>
-      <c r="M162" s="23"/>
+      <c r="B162" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C162" s="37" t="s">
+        <v>526</v>
+      </c>
+      <c r="D162" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="E162" s="24" t="s">
+        <v>528</v>
+      </c>
+      <c r="F162" s="24" t="s">
+        <v>527</v>
+      </c>
+      <c r="G162" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="H162" s="24" t="s">
+        <v>530</v>
+      </c>
+      <c r="I162" s="24" t="s">
+        <v>529</v>
+      </c>
+      <c r="J162" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K162" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="L162" s="21">
+        <v>2018</v>
+      </c>
+      <c r="M162" s="23" t="s">
+        <v>533</v>
+      </c>
       <c r="N162" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Concha-Meyer, A. et al., Differenzmethode, 2018, S. 1868-1869.</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" s="21">
         <v>162</v>
       </c>
-      <c r="B163" s="21"/>
-      <c r="C163" s="24"/>
-      <c r="D163" s="24"/>
-      <c r="E163" s="24"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="21"/>
-      <c r="H163" s="24"/>
-      <c r="I163" s="24"/>
-      <c r="J163" s="25"/>
-      <c r="K163" s="24"/>
-      <c r="L163" s="21"/>
-      <c r="M163" s="23"/>
+      <c r="B163" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C163" s="37" t="s">
+        <v>555</v>
+      </c>
+      <c r="D163" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="E163" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="F163" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="G163" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="H163" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="I163" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="J163" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K163" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="L163" s="21">
+        <v>2000</v>
+      </c>
+      <c r="M163" s="23" t="s">
+        <v>557</v>
+      </c>
       <c r="N163" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Triggs, B. et al., bundle adjustment, 2000, S. 298-300.</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" s="21">
         <v>163</v>
       </c>
-      <c r="B164" s="21"/>
-      <c r="C164" s="24"/>
-      <c r="D164" s="24"/>
-      <c r="E164" s="24"/>
-      <c r="F164" s="21"/>
-      <c r="G164" s="21"/>
-      <c r="H164" s="24"/>
-      <c r="I164" s="24"/>
-      <c r="J164" s="25"/>
-      <c r="K164" s="24"/>
-      <c r="L164" s="21"/>
-      <c r="M164" s="23"/>
+      <c r="B164" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C164" s="37" t="s">
+        <v>555</v>
+      </c>
+      <c r="D164" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="E164" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="F164" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="G164" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="H164" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="I164" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="J164" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K164" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="L164" s="21">
+        <v>2000</v>
+      </c>
+      <c r="M164" s="23" t="s">
+        <v>557</v>
+      </c>
       <c r="N164" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Triggs, B. et al., bundle adjustment, 2000, S. 298-300.</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" s="14">
         <v>164</v>
       </c>
-      <c r="B165" s="21"/>
-      <c r="C165" s="24"/>
-      <c r="D165" s="24"/>
-      <c r="E165" s="24"/>
-      <c r="F165" s="21"/>
-      <c r="G165" s="21"/>
-      <c r="H165" s="24"/>
-      <c r="I165" s="24"/>
-      <c r="J165" s="25"/>
-      <c r="K165" s="24"/>
-      <c r="L165" s="21"/>
-      <c r="M165" s="23"/>
+      <c r="B165" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C165" s="37" t="s">
+        <v>555</v>
+      </c>
+      <c r="D165" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="E165" s="24" t="s">
+        <v>550</v>
+      </c>
+      <c r="F165" s="24" t="s">
+        <v>558</v>
+      </c>
+      <c r="G165" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="H165" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="I165" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="J165" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K165" s="24" t="s">
+        <v>554</v>
+      </c>
+      <c r="L165" s="21">
+        <v>2000</v>
+      </c>
+      <c r="M165" s="23" t="s">
+        <v>559</v>
+      </c>
       <c r="N165" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Triggs, B. et al., bundle adjustment, 2000, S. 299, 304-305.</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" s="21">
         <v>165</v>
       </c>
-      <c r="B166" s="21"/>
-      <c r="C166" s="24"/>
-      <c r="D166" s="24"/>
-      <c r="E166" s="24"/>
-      <c r="F166" s="21"/>
-      <c r="G166" s="21"/>
-      <c r="H166" s="24"/>
-      <c r="I166" s="24"/>
-      <c r="J166" s="25"/>
-      <c r="K166" s="24"/>
-      <c r="L166" s="21"/>
-      <c r="M166" s="23"/>
+      <c r="B166" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C166" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="D166" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="E166" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="F166" s="24" t="s">
+        <v>563</v>
+      </c>
+      <c r="G166" s="24" t="s">
+        <v>564</v>
+      </c>
+      <c r="H166" s="24" t="s">
+        <v>566</v>
+      </c>
+      <c r="I166" s="24" t="s">
+        <v>565</v>
+      </c>
+      <c r="J166" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K166" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="L166" s="21">
+        <v>2006</v>
+      </c>
+      <c r="M166" s="23" t="s">
+        <v>569</v>
+      </c>
       <c r="N166" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Bay, H. et al., SURF, 2006, S. 404-417.</v>
+      </c>
+      <c r="O166" s="5" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" s="21">
         <v>166</v>
       </c>
-      <c r="B167" s="21"/>
-      <c r="C167" s="24"/>
-      <c r="D167" s="24"/>
-      <c r="E167" s="24"/>
-      <c r="F167" s="21"/>
-      <c r="G167" s="21"/>
-      <c r="H167" s="24"/>
-      <c r="I167" s="24"/>
-      <c r="J167" s="25"/>
-      <c r="K167" s="24"/>
-      <c r="L167" s="21"/>
-      <c r="M167" s="23"/>
+      <c r="B167" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C167" s="37" t="s">
+        <v>560</v>
+      </c>
+      <c r="D167" s="24" t="s">
+        <v>561</v>
+      </c>
+      <c r="E167" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="F167" s="24" t="s">
+        <v>563</v>
+      </c>
+      <c r="G167" s="24" t="s">
+        <v>564</v>
+      </c>
+      <c r="H167" s="24" t="s">
+        <v>566</v>
+      </c>
+      <c r="I167" s="24" t="s">
+        <v>565</v>
+      </c>
+      <c r="J167" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K167" s="24" t="s">
+        <v>567</v>
+      </c>
+      <c r="L167" s="21">
+        <v>2006</v>
+      </c>
+      <c r="M167" s="23" t="s">
+        <v>570</v>
+      </c>
       <c r="N167" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Bay, H. et al., SURF, 2006, S. 404.</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="14">
         <v>167</v>
       </c>
-      <c r="B168" s="21"/>
-      <c r="C168" s="24"/>
-      <c r="D168" s="24"/>
-      <c r="E168" s="24"/>
-      <c r="F168" s="21"/>
-      <c r="G168" s="21"/>
-      <c r="H168" s="24"/>
-      <c r="I168" s="24"/>
-      <c r="J168" s="25"/>
-      <c r="K168" s="24"/>
-      <c r="L168" s="21"/>
-      <c r="M168" s="23"/>
+      <c r="B168" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C168" s="37" t="s">
+        <v>577</v>
+      </c>
+      <c r="D168" s="24" t="s">
+        <v>572</v>
+      </c>
+      <c r="E168" s="47" t="s">
+        <v>571</v>
+      </c>
+      <c r="F168" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="G168" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="H168" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="I168" s="24" t="s">
+        <v>573</v>
+      </c>
+      <c r="J168" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K168" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="L168" s="21">
+        <v>2021</v>
+      </c>
+      <c r="M168" s="23" t="s">
+        <v>579</v>
+      </c>
       <c r="N168" s="17" t="str">
         <f t="shared" si="5"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Bansal, M. et al., SIFT vs. SURF, 2021, S. 18843-18844.</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="21">
         <v>168</v>
       </c>
-      <c r="B169" s="21"/>
-      <c r="C169" s="24"/>
-      <c r="D169" s="24"/>
-      <c r="E169" s="24"/>
-      <c r="F169" s="21"/>
-      <c r="G169" s="21"/>
-      <c r="H169" s="24"/>
-      <c r="I169" s="24"/>
-      <c r="J169" s="25"/>
-      <c r="K169" s="24"/>
-      <c r="L169" s="21"/>
-      <c r="M169" s="23"/>
+      <c r="B169" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C169" s="37" t="s">
+        <v>577</v>
+      </c>
+      <c r="D169" s="24" t="s">
+        <v>572</v>
+      </c>
+      <c r="E169" s="47" t="s">
+        <v>571</v>
+      </c>
+      <c r="F169" s="24" t="s">
+        <v>576</v>
+      </c>
+      <c r="G169" s="24" t="s">
+        <v>575</v>
+      </c>
+      <c r="H169" s="24" t="s">
+        <v>574</v>
+      </c>
+      <c r="I169" s="24" t="s">
+        <v>573</v>
+      </c>
+      <c r="J169" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K169" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="L169" s="21">
+        <v>2021</v>
+      </c>
+      <c r="M169" s="23" t="s">
+        <v>579</v>
+      </c>
       <c r="N169" s="17" t="str">
         <f t="shared" ref="N169:N202" si="6">"Vgl. "&amp;H169&amp;", "&amp;F169&amp;", "&amp;L169&amp;", S. "&amp;M169&amp;"."</f>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Bansal, M. et al., SIFT vs. SURF, 2021, S. 18843-18844.</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" s="21">
         <v>169</v>
       </c>
-      <c r="B170" s="21"/>
-      <c r="C170" s="24"/>
-      <c r="D170" s="24"/>
-      <c r="E170" s="24"/>
-      <c r="F170" s="21"/>
-      <c r="G170" s="21"/>
-      <c r="H170" s="24"/>
-      <c r="I170" s="24"/>
-      <c r="J170" s="25"/>
-      <c r="K170" s="24"/>
-      <c r="L170" s="21"/>
-      <c r="M170" s="23"/>
+      <c r="B170" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C170" s="37" t="s">
+        <v>581</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="E170" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F170" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="G170" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="H170" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="I170" s="24" t="s">
+        <v>585</v>
+      </c>
+      <c r="J170" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K170" s="24" t="s">
+        <v>587</v>
+      </c>
+      <c r="L170" s="21">
+        <v>2010</v>
+      </c>
+      <c r="M170" s="23" t="s">
+        <v>588</v>
+      </c>
       <c r="N170" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Furukawa, Y.; Ponce, J., PMVS, 2010, S. 1-8.</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" s="14">
         <v>170</v>
       </c>
-      <c r="B171" s="21"/>
-      <c r="C171" s="24"/>
-      <c r="D171" s="24"/>
-      <c r="E171" s="24"/>
-      <c r="F171" s="21"/>
-      <c r="G171" s="21"/>
-      <c r="H171" s="24"/>
-      <c r="I171" s="24"/>
-      <c r="J171" s="25"/>
-      <c r="K171" s="24"/>
-      <c r="L171" s="21"/>
-      <c r="M171" s="23"/>
+      <c r="B171" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" s="37" t="s">
+        <v>581</v>
+      </c>
+      <c r="D171" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="E171" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F171" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="G171" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="H171" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="I171" s="24" t="s">
+        <v>585</v>
+      </c>
+      <c r="J171" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K171" s="24" t="s">
+        <v>587</v>
+      </c>
+      <c r="L171" s="21">
+        <v>2010</v>
+      </c>
+      <c r="M171" s="23" t="s">
+        <v>264</v>
+      </c>
       <c r="N171" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Furukawa, Y.; Ponce, J., PMVS, 2010, S. 1-3.</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" s="21">
         <v>171</v>
       </c>
-      <c r="B172" s="21"/>
-      <c r="C172" s="24"/>
-      <c r="D172" s="24"/>
-      <c r="E172" s="24"/>
-      <c r="F172" s="21"/>
-      <c r="G172" s="21"/>
-      <c r="H172" s="24"/>
-      <c r="I172" s="24"/>
-      <c r="J172" s="25"/>
-      <c r="K172" s="24"/>
-      <c r="L172" s="21"/>
-      <c r="M172" s="23"/>
+      <c r="B172" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C172" s="37" t="s">
+        <v>581</v>
+      </c>
+      <c r="D172" s="24" t="s">
+        <v>583</v>
+      </c>
+      <c r="E172" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F172" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="G172" s="24" t="s">
+        <v>584</v>
+      </c>
+      <c r="H172" s="24" t="s">
+        <v>586</v>
+      </c>
+      <c r="I172" s="24" t="s">
+        <v>585</v>
+      </c>
+      <c r="J172" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K172" s="24" t="s">
+        <v>587</v>
+      </c>
+      <c r="L172" s="21">
+        <v>2010</v>
+      </c>
+      <c r="M172" s="23" t="s">
+        <v>589</v>
+      </c>
       <c r="N172" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Furukawa, Y.; Ponce, J., PMVS, 2010, S. 1, 3-4.</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" s="21">
         <v>172</v>
       </c>
-      <c r="B173" s="21"/>
-      <c r="C173" s="24"/>
-      <c r="D173" s="24"/>
-      <c r="E173" s="24"/>
-      <c r="F173" s="21"/>
-      <c r="G173" s="21"/>
-      <c r="H173" s="24"/>
-      <c r="I173" s="24"/>
-      <c r="J173" s="25"/>
-      <c r="K173" s="24"/>
-      <c r="L173" s="21"/>
-      <c r="M173" s="23"/>
+      <c r="B173" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C173" s="37" t="s">
+        <v>604</v>
+      </c>
+      <c r="D173" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="E173" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="F173" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="G173" s="24" t="s">
+        <v>600</v>
+      </c>
+      <c r="H173" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="I173" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="J173" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K173" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="L173" s="21">
+        <v>2020</v>
+      </c>
+      <c r="M173" s="23" t="s">
+        <v>609</v>
+      </c>
       <c r="N173" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Wang, X. et al., 3D-DCGAN, 2020, S. 170355-170356.</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" s="14">
         <v>173</v>
       </c>
-      <c r="B174" s="21"/>
-      <c r="C174" s="24"/>
-      <c r="D174" s="24"/>
-      <c r="E174" s="24"/>
-      <c r="F174" s="21"/>
-      <c r="G174" s="21"/>
-      <c r="H174" s="24"/>
-      <c r="I174" s="24"/>
-      <c r="J174" s="25"/>
-      <c r="K174" s="24"/>
-      <c r="L174" s="21"/>
-      <c r="M174" s="23"/>
+      <c r="B174" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C174" s="37" t="s">
+        <v>590</v>
+      </c>
+      <c r="D174" s="24" t="s">
+        <v>591</v>
+      </c>
+      <c r="E174" s="24" t="s">
+        <v>592</v>
+      </c>
+      <c r="F174" s="24" t="s">
+        <v>593</v>
+      </c>
+      <c r="G174" s="24" t="s">
+        <v>594</v>
+      </c>
+      <c r="H174" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="I174" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="J174" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K174" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="L174" s="21">
+        <v>2022</v>
+      </c>
+      <c r="M174" s="23" t="s">
+        <v>261</v>
+      </c>
       <c r="N174" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Ren, Y. et al., hole filling methods, 2022, S. 1.</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="21">
         <v>174</v>
       </c>
-      <c r="B175" s="21"/>
-      <c r="C175" s="24"/>
-      <c r="D175" s="24"/>
-      <c r="E175" s="24"/>
-      <c r="F175" s="21"/>
-      <c r="G175" s="21"/>
-      <c r="H175" s="24"/>
-      <c r="I175" s="24"/>
-      <c r="J175" s="25"/>
-      <c r="K175" s="24"/>
-      <c r="L175" s="21"/>
-      <c r="M175" s="23"/>
+      <c r="B175" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C175" s="37" t="s">
+        <v>604</v>
+      </c>
+      <c r="D175" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="E175" s="24" t="s">
+        <v>602</v>
+      </c>
+      <c r="F175" s="24" t="s">
+        <v>601</v>
+      </c>
+      <c r="G175" s="24" t="s">
+        <v>600</v>
+      </c>
+      <c r="H175" s="24" t="s">
+        <v>599</v>
+      </c>
+      <c r="I175" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="J175" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K175" s="24" t="s">
+        <v>605</v>
+      </c>
+      <c r="L175" s="21">
+        <v>2020</v>
+      </c>
+      <c r="M175" s="23" t="s">
+        <v>606</v>
+      </c>
       <c r="N175" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Wang, X. et al., 3D-DCGAN, 2020, S. 170355-170363.</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" s="21">
         <v>175</v>
       </c>
-      <c r="B176" s="21"/>
-      <c r="C176" s="24"/>
-      <c r="D176" s="24"/>
-      <c r="E176" s="24"/>
-      <c r="F176" s="21"/>
-      <c r="G176" s="21"/>
-      <c r="H176" s="24"/>
-      <c r="I176" s="24"/>
-      <c r="J176" s="25"/>
-      <c r="K176" s="24"/>
-      <c r="L176" s="21"/>
-      <c r="M176" s="23"/>
+      <c r="B176" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C176" s="37" t="s">
+        <v>590</v>
+      </c>
+      <c r="D176" s="24" t="s">
+        <v>591</v>
+      </c>
+      <c r="E176" s="24" t="s">
+        <v>592</v>
+      </c>
+      <c r="F176" s="24" t="s">
+        <v>608</v>
+      </c>
+      <c r="G176" s="24" t="s">
+        <v>594</v>
+      </c>
+      <c r="H176" s="24" t="s">
+        <v>597</v>
+      </c>
+      <c r="I176" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="J176" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K176" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="L176" s="21">
+        <v>2022</v>
+      </c>
+      <c r="M176" s="23" t="s">
+        <v>607</v>
+      </c>
       <c r="N176" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Ren, Y. et al., MU-GAN, 2022, S. 1-14.</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="14">
         <v>176</v>
       </c>
-      <c r="B177" s="21"/>
-      <c r="C177" s="24"/>
-      <c r="D177" s="24"/>
-      <c r="E177" s="24"/>
-      <c r="F177" s="21"/>
-      <c r="G177" s="21"/>
-      <c r="H177" s="24"/>
-      <c r="I177" s="24"/>
-      <c r="J177" s="25"/>
-      <c r="K177" s="24"/>
-      <c r="L177" s="21"/>
-      <c r="M177" s="23"/>
+      <c r="B177" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" s="37" t="s">
+        <v>610</v>
+      </c>
+      <c r="D177" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E177" s="24" t="s">
+        <v>611</v>
+      </c>
+      <c r="F177" s="24" t="s">
+        <v>611</v>
+      </c>
+      <c r="G177" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H177" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I177" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J177" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K177" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L177" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M177" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N177" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., WWDC21, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="21">
         <v>177</v>
       </c>
-      <c r="B178" s="21"/>
-      <c r="C178" s="24"/>
-      <c r="D178" s="24"/>
-      <c r="E178" s="24"/>
-      <c r="F178" s="21"/>
-      <c r="G178" s="21"/>
-      <c r="H178" s="24"/>
-      <c r="I178" s="24"/>
-      <c r="J178" s="25"/>
-      <c r="K178" s="24"/>
-      <c r="L178" s="21"/>
-      <c r="M178" s="23"/>
+      <c r="B178" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C178" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D178" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E178" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F178" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G178" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H178" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I178" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J178" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K178" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L178" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M178" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N178" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" s="21">
         <v>178</v>
       </c>
-      <c r="B179" s="21"/>
-      <c r="C179" s="24"/>
-      <c r="D179" s="24"/>
-      <c r="E179" s="24"/>
-      <c r="F179" s="21"/>
-      <c r="G179" s="21"/>
-      <c r="H179" s="24"/>
-      <c r="I179" s="24"/>
-      <c r="J179" s="25"/>
-      <c r="K179" s="24"/>
-      <c r="L179" s="21"/>
-      <c r="M179" s="23"/>
+      <c r="B179" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C179" s="37" t="s">
+        <v>615</v>
+      </c>
+      <c r="D179" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E179" s="24" t="s">
+        <v>616</v>
+      </c>
+      <c r="F179" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="G179" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H179" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I179" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J179" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K179" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L179" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M179" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N179" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., AR, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" s="14">
         <v>179</v>
       </c>
-      <c r="B180" s="21"/>
-      <c r="C180" s="24"/>
-      <c r="D180" s="24"/>
-      <c r="E180" s="24"/>
-      <c r="F180" s="21"/>
-      <c r="G180" s="21"/>
-      <c r="H180" s="24"/>
-      <c r="I180" s="24"/>
-      <c r="J180" s="25"/>
-      <c r="K180" s="24"/>
-      <c r="L180" s="21"/>
-      <c r="M180" s="23"/>
+      <c r="B180" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C180" s="37" t="s">
+        <v>623</v>
+      </c>
+      <c r="D180" s="24" t="s">
+        <v>622</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>618</v>
+      </c>
+      <c r="F180" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="G180" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="H180" s="24" t="s">
+        <v>620</v>
+      </c>
+      <c r="I180" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="J180" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K180" s="24" t="s">
+        <v>624</v>
+      </c>
+      <c r="L180" s="21">
+        <v>1968</v>
+      </c>
+      <c r="M180" s="23" t="s">
+        <v>626</v>
+      </c>
       <c r="N180" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Sutherland, I., AR, 1968, S. 757-764.</v>
+      </c>
+      <c r="O180" s="55" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" s="21">
         <v>180</v>
       </c>
-      <c r="B181" s="21"/>
-      <c r="C181" s="24"/>
-      <c r="D181" s="24"/>
-      <c r="E181" s="24"/>
-      <c r="F181" s="21"/>
-      <c r="G181" s="21"/>
-      <c r="H181" s="24"/>
-      <c r="I181" s="24"/>
-      <c r="J181" s="25"/>
-      <c r="K181" s="24"/>
-      <c r="L181" s="21"/>
-      <c r="M181" s="23"/>
+      <c r="B181" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C181" s="37" t="s">
+        <v>628</v>
+      </c>
+      <c r="D181" s="24" t="s">
+        <v>627</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="F181" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="G181" s="24" t="s">
+        <v>630</v>
+      </c>
+      <c r="H181" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="I181" s="24" t="s">
+        <v>631</v>
+      </c>
+      <c r="J181" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K181" s="24" t="s">
+        <v>633</v>
+      </c>
+      <c r="L181" s="21">
+        <v>2022</v>
+      </c>
+      <c r="M181" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="N181" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Arena, F. et al., AR, 2022, S. 1-2.</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" s="21">
         <v>181</v>
       </c>
-      <c r="B182" s="21"/>
-      <c r="C182" s="24"/>
-      <c r="D182" s="24"/>
-      <c r="E182" s="24"/>
-      <c r="F182" s="21"/>
-      <c r="G182" s="21"/>
-      <c r="H182" s="24"/>
-      <c r="I182" s="24"/>
-      <c r="J182" s="25"/>
-      <c r="K182" s="24"/>
-      <c r="L182" s="21"/>
-      <c r="M182" s="23"/>
+      <c r="B182" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C182" s="37" t="s">
+        <v>634</v>
+      </c>
+      <c r="D182" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E182" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="F182" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G182" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H182" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I182" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J182" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K182" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L182" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M182" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N182" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" s="14">
         <v>182</v>
       </c>
-      <c r="B183" s="21"/>
-      <c r="C183" s="24"/>
-      <c r="D183" s="24"/>
-      <c r="E183" s="24"/>
-      <c r="F183" s="21"/>
-      <c r="G183" s="21"/>
-      <c r="H183" s="24"/>
-      <c r="I183" s="24"/>
-      <c r="J183" s="25"/>
-      <c r="K183" s="24"/>
-      <c r="L183" s="21"/>
-      <c r="M183" s="23"/>
+      <c r="B183" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" s="37" t="s">
+        <v>634</v>
+      </c>
+      <c r="D183" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E183" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="F183" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G183" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H183" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I183" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J183" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K183" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L183" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M183" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N183" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" s="21">
         <v>183</v>
       </c>
-      <c r="B184" s="21"/>
-      <c r="C184" s="24"/>
-      <c r="D184" s="24"/>
-      <c r="E184" s="24"/>
-      <c r="F184" s="21"/>
-      <c r="G184" s="21"/>
-      <c r="H184" s="24"/>
-      <c r="I184" s="24"/>
-      <c r="J184" s="25"/>
-      <c r="K184" s="24"/>
-      <c r="L184" s="21"/>
-      <c r="M184" s="23"/>
+      <c r="B184" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C184" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D184" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E184" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F184" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G184" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H184" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I184" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J184" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K184" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L184" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M184" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N184" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" s="21">
         <v>184</v>
       </c>
-      <c r="B185" s="21"/>
-      <c r="C185" s="24"/>
-      <c r="D185" s="24"/>
-      <c r="E185" s="24"/>
-      <c r="F185" s="21"/>
-      <c r="G185" s="21"/>
-      <c r="H185" s="24"/>
-      <c r="I185" s="24"/>
-      <c r="J185" s="25"/>
-      <c r="K185" s="24"/>
-      <c r="L185" s="21"/>
-      <c r="M185" s="23"/>
+      <c r="B185" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C185" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D185" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E185" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F185" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G185" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H185" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I185" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J185" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K185" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L185" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M185" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N185" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" s="14">
         <v>185</v>
       </c>
-      <c r="B186" s="21"/>
-      <c r="C186" s="24"/>
-      <c r="D186" s="24"/>
-      <c r="E186" s="24"/>
-      <c r="F186" s="21"/>
-      <c r="G186" s="21"/>
-      <c r="H186" s="24"/>
-      <c r="I186" s="24"/>
-      <c r="J186" s="25"/>
-      <c r="K186" s="24"/>
-      <c r="L186" s="21"/>
-      <c r="M186" s="23"/>
+      <c r="B186" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C186" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D186" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E186" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F186" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G186" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H186" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I186" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J186" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K186" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L186" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M186" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N186" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" s="21">
         <v>186</v>
       </c>
-      <c r="B187" s="21"/>
-      <c r="C187" s="24"/>
-      <c r="D187" s="24"/>
-      <c r="E187" s="24"/>
-      <c r="F187" s="21"/>
-      <c r="G187" s="21"/>
-      <c r="H187" s="24"/>
-      <c r="I187" s="24"/>
-      <c r="J187" s="25"/>
-      <c r="K187" s="24"/>
-      <c r="L187" s="21"/>
-      <c r="M187" s="23"/>
+      <c r="B187" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C187" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D187" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E187" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F187" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G187" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H187" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I187" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J187" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K187" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L187" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M187" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N187" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" s="21">
         <v>187</v>
       </c>
-      <c r="B188" s="21"/>
-      <c r="C188" s="24"/>
-      <c r="D188" s="24"/>
-      <c r="E188" s="24"/>
-      <c r="F188" s="21"/>
-      <c r="G188" s="21"/>
-      <c r="H188" s="24"/>
-      <c r="I188" s="24"/>
-      <c r="J188" s="25"/>
-      <c r="K188" s="24"/>
-      <c r="L188" s="21"/>
-      <c r="M188" s="23"/>
+      <c r="B188" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C188" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D188" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E188" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F188" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G188" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H188" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I188" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J188" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K188" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L188" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M188" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N188" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" s="14">
         <v>188</v>
       </c>
-      <c r="B189" s="21"/>
-      <c r="C189" s="24"/>
-      <c r="D189" s="24"/>
-      <c r="E189" s="24"/>
-      <c r="F189" s="21"/>
-      <c r="G189" s="21"/>
-      <c r="H189" s="24"/>
-      <c r="I189" s="24"/>
-      <c r="J189" s="25"/>
-      <c r="K189" s="24"/>
-      <c r="L189" s="21"/>
-      <c r="M189" s="23"/>
+      <c r="B189" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C189" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D189" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E189" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F189" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G189" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H189" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I189" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J189" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K189" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L189" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M189" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N189" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" s="21">
         <v>189</v>
       </c>
-      <c r="B190" s="21"/>
-      <c r="C190" s="24"/>
-      <c r="D190" s="24"/>
-      <c r="E190" s="24"/>
-      <c r="F190" s="21"/>
-      <c r="G190" s="21"/>
-      <c r="H190" s="24"/>
-      <c r="I190" s="24"/>
-      <c r="J190" s="25"/>
-      <c r="K190" s="24"/>
-      <c r="L190" s="21"/>
-      <c r="M190" s="23"/>
+      <c r="B190" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C190" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D190" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E190" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F190" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G190" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H190" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I190" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J190" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K190" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L190" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M190" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N190" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" s="21">
         <v>190</v>
       </c>
-      <c r="B191" s="21"/>
-      <c r="C191" s="24"/>
-      <c r="D191" s="24"/>
-      <c r="E191" s="24"/>
-      <c r="F191" s="21"/>
-      <c r="G191" s="21"/>
-      <c r="H191" s="24"/>
-      <c r="I191" s="24"/>
-      <c r="J191" s="25"/>
-      <c r="K191" s="24"/>
-      <c r="L191" s="21"/>
-      <c r="M191" s="23"/>
+      <c r="B191" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C191" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D191" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E191" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F191" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G191" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H191" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I191" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J191" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K191" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L191" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M191" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N191" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
-      </c>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" s="14">
         <v>191</v>
       </c>
-      <c r="B192" s="21"/>
-      <c r="C192" s="24"/>
-      <c r="D192" s="24"/>
-      <c r="E192" s="24"/>
-      <c r="F192" s="21"/>
-      <c r="G192" s="21"/>
-      <c r="H192" s="24"/>
-      <c r="I192" s="24"/>
-      <c r="J192" s="25"/>
-      <c r="K192" s="24"/>
-      <c r="L192" s="21"/>
-      <c r="M192" s="23"/>
+      <c r="B192" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C192" s="37" t="s">
+        <v>613</v>
+      </c>
+      <c r="D192" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E192" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F192" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="G192" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H192" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I192" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J192" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="K192" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L192" s="21">
+        <v>2023</v>
+      </c>
+      <c r="M192" s="23" t="s">
+        <v>521</v>
+      </c>
       <c r="N192" s="17" t="str">
         <f t="shared" si="6"/>
-        <v>Vgl. , , , S. .</v>
+        <v>Vgl. Apple Inc., RealityKit Object Capture, 2023, S. o. S..</v>
       </c>
     </row>
     <row r="193" spans="1:14" x14ac:dyDescent="0.2">
@@ -10267,6 +11654,46 @@
     <hyperlink ref="C150" r:id="rId147" xr:uid="{DA666082-F26D-6A42-B7DF-3A3773D141EE}"/>
     <hyperlink ref="C151" r:id="rId148" xr:uid="{6E1845B6-4C45-B240-92C2-C9E177980429}"/>
     <hyperlink ref="C152" r:id="rId149" xr:uid="{0B9295B3-1F82-3E41-BB00-1AD614A66DB0}"/>
+    <hyperlink ref="C153" r:id="rId150" xr:uid="{E54EA9E0-C4EA-8242-A765-EC84D3E3A048}"/>
+    <hyperlink ref="C156" r:id="rId151" xr:uid="{CECDAC76-BFA6-9649-9F6C-1275D55950DD}"/>
+    <hyperlink ref="C155" r:id="rId152" xr:uid="{593CA1D9-8B27-DD49-9EDB-DE4FE444FA88}"/>
+    <hyperlink ref="C154" r:id="rId153" xr:uid="{38A42C96-E847-674C-850C-EBEAB933D601}"/>
+    <hyperlink ref="C159" r:id="rId154" xr:uid="{6F6FF947-047F-7C41-88B3-65286682D3AE}"/>
+    <hyperlink ref="C157" r:id="rId155" xr:uid="{4CF9D765-7499-864E-8091-24A550C2F96F}"/>
+    <hyperlink ref="C158" r:id="rId156" xr:uid="{D09399FF-90C2-274B-9127-1241D3F2A96F}"/>
+    <hyperlink ref="C160" r:id="rId157" xr:uid="{29C29B04-FC6A-FA4C-838D-5C56C7FA579D}"/>
+    <hyperlink ref="C162" r:id="rId158" xr:uid="{0D1BF240-A589-DD46-AB4F-D5FB8CAAE3DC}"/>
+    <hyperlink ref="C161" r:id="rId159" xr:uid="{0A3E6E3D-121A-7646-A301-0DC4A5483518}"/>
+    <hyperlink ref="C163" r:id="rId160" location="citeas" xr:uid="{D0CB4034-BD6B-E146-8697-EE26E18FFFE9}"/>
+    <hyperlink ref="C164" r:id="rId161" location="citeas" xr:uid="{469FFD05-E43C-5B46-A15C-06225E5D5024}"/>
+    <hyperlink ref="C165" r:id="rId162" location="citeas" xr:uid="{87B58E25-7AB4-A440-85D2-6C40BAA3425A}"/>
+    <hyperlink ref="C166" r:id="rId163" xr:uid="{BE62531B-E371-6542-84B6-363A60E44A57}"/>
+    <hyperlink ref="C167" r:id="rId164" xr:uid="{6FBF000E-C4B0-7E41-9999-2DA7A2A8FC3A}"/>
+    <hyperlink ref="C168" r:id="rId165" xr:uid="{55C84FDA-174B-E841-AA6D-A81DD65534ED}"/>
+    <hyperlink ref="C169" r:id="rId166" xr:uid="{70D01F60-433A-3F43-A56E-2E02D6F45870}"/>
+    <hyperlink ref="C170" r:id="rId167" xr:uid="{F3971876-1FC8-0B45-BF8E-C4812B651555}"/>
+    <hyperlink ref="C171" r:id="rId168" xr:uid="{CCFB26C5-B7F3-2745-9412-7B5BF5794848}"/>
+    <hyperlink ref="C172" r:id="rId169" xr:uid="{A140097F-DC7A-DD41-9A5C-22F61542BDF0}"/>
+    <hyperlink ref="C174" r:id="rId170" xr:uid="{1BB87E92-5C5A-4B49-ABFC-B300C3FB49DF}"/>
+    <hyperlink ref="C175" r:id="rId171" xr:uid="{E5A96435-2B65-1C4B-BC01-C7A2F3B6CBBE}"/>
+    <hyperlink ref="C176" r:id="rId172" xr:uid="{126BB29F-4D1F-1649-8C5D-DC5DAB5302C0}"/>
+    <hyperlink ref="C173" r:id="rId173" xr:uid="{47C23292-AC8D-AC48-8BE4-6DEA26C292C7}"/>
+    <hyperlink ref="C177" r:id="rId174" xr:uid="{46CDA66F-1188-E141-BB82-2713DF20651D}"/>
+    <hyperlink ref="C178" r:id="rId175" xr:uid="{9C50888C-D413-EE4C-9F84-15D7B6E33D40}"/>
+    <hyperlink ref="C179" r:id="rId176" xr:uid="{75EB647A-AE8E-0240-B507-BEF427BBE2F8}"/>
+    <hyperlink ref="C180" r:id="rId177" xr:uid="{4D117CD9-F7A8-AC42-A63A-194013A4122E}"/>
+    <hyperlink ref="C181" r:id="rId178" xr:uid="{549EA58B-D42F-DD47-BDB4-A2F91E82EEF2}"/>
+    <hyperlink ref="C182" r:id="rId179" xr:uid="{935C9F91-9341-3740-BAD9-82ABDDE8FB36}"/>
+    <hyperlink ref="C183" r:id="rId180" xr:uid="{0542D0C3-4E9E-884D-B8B8-977C3F5FF3A3}"/>
+    <hyperlink ref="C184" r:id="rId181" xr:uid="{DDA39FC2-0F09-F142-9CE6-C6FC4F7994CE}"/>
+    <hyperlink ref="C185" r:id="rId182" xr:uid="{D35AA936-4345-9346-A674-231B5B02F908}"/>
+    <hyperlink ref="C186" r:id="rId183" xr:uid="{BBEAC91B-4FDB-5947-BD92-23B98725E477}"/>
+    <hyperlink ref="C187" r:id="rId184" xr:uid="{FE919FD4-4438-1E4B-B095-D8B0ED810ACD}"/>
+    <hyperlink ref="C188" r:id="rId185" xr:uid="{BB168FB2-044C-D948-AF09-8DE988FDE904}"/>
+    <hyperlink ref="C189" r:id="rId186" xr:uid="{3B0FDD7F-59E4-8F49-883C-58094FFF77AC}"/>
+    <hyperlink ref="C190" r:id="rId187" xr:uid="{662A0FB8-DF8B-074A-A351-CC58E416740D}"/>
+    <hyperlink ref="C191" r:id="rId188" xr:uid="{121DF433-ECA7-EA47-8E80-CF6833C1A7F6}"/>
+    <hyperlink ref="C192" r:id="rId189" xr:uid="{53EDC8CE-2062-384B-BB8D-D56A8FD9B829}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10275,10 +11702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C48A7A-8BD0-CF4B-BE42-71F225EF32B1}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10291,9 +11718,11 @@
     <col min="8" max="8" width="30.33203125" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="40.5" customWidth="1"/>
+    <col min="13" max="13" width="16.5" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10330,18 +11759,24 @@
       <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="51" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>101</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -10367,17 +11802,17 @@
       </c>
       <c r="L2" s="40"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="10" t="s">
         <v>270</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -10403,17 +11838,17 @@
       </c>
       <c r="L3" s="40"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>284</v>
       </c>
       <c r="E4" s="19" t="s">
@@ -10439,17 +11874,17 @@
       </c>
       <c r="L4" s="40"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="10" t="s">
         <v>318</v>
       </c>
       <c r="E5" s="9" t="s">
@@ -10477,17 +11912,17 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="10" t="s">
         <v>418</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>419</v>
       </c>
       <c r="E6" s="9" t="s">
@@ -10515,77 +11950,155 @@
         <v>420</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="40"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>508</v>
+      </c>
+      <c r="G7" s="38" t="s">
+        <v>509</v>
+      </c>
+      <c r="H7" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="I7" s="12">
+        <v>2021</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="L7" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>511</v>
+      </c>
+      <c r="N7" s="52" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="40"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>472</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>473</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>479</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1981</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="K8" s="2">
+        <v>166</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="40"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>539</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>535</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>536</v>
+      </c>
+      <c r="I9" s="12">
+        <v>2017</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="K9" s="2">
+        <v>36</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" t="s">
+        <v>541</v>
+      </c>
+      <c r="N9" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="9"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="12"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="40"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="9"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -10595,7 +12108,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="40"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -10611,7 +12124,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="40"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -10627,7 +12140,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -10643,7 +12156,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="40"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -10659,7 +12172,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="40"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -10899,6 +12412,9 @@
     <hyperlink ref="E4" r:id="rId4" xr:uid="{DA54CC3D-E2C6-814C-8135-ED7908FDC10E}"/>
     <hyperlink ref="E5" r:id="rId5" xr:uid="{CD036F67-6E04-E043-A191-F6F8C841A3A0}"/>
     <hyperlink ref="E6" r:id="rId6" xr:uid="{972E71EE-38C7-2848-B599-01D8A0B345FB}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{50ADBD92-83B1-2045-A287-23814659131C}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{A391AB37-BA15-5346-98D0-9DA0F9B9773A}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{1DF39F88-C72C-BB44-B81F-7071CCD22EAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11401,8 +12917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AFC829A-15CB-4349-B67F-7F5156541E53}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A6" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11804,33 +13320,77 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>519</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>518</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>520</v>
+      </c>
+      <c r="G11" s="12">
+        <v>2023</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>464</v>
+      </c>
+      <c r="E12" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>466</v>
+      </c>
+      <c r="G12" s="12">
+        <v>2021</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>470</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="K12" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -12117,6 +13677,8 @@
     <hyperlink ref="L8" r:id="rId7" xr:uid="{9D945A69-59B2-844C-BB89-267FDD954506}"/>
     <hyperlink ref="L9" r:id="rId8" location="citeas" xr:uid="{E93028B3-D238-D84E-856F-FE78DE64030A}"/>
     <hyperlink ref="L10" r:id="rId9" location="citeas" xr:uid="{CAEA1B2E-B154-6643-A49E-03F3EC750188}"/>
+    <hyperlink ref="L12" r:id="rId10" xr:uid="{050392BF-DD43-FC4E-BFDA-AD8D5D5B0855}"/>
+    <hyperlink ref="L11" r:id="rId11" xr:uid="{65CE9CE3-F67C-7045-A1B6-F858124A3CA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>